<commit_message>
jn: realizados 3 diccionarios
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_18.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_18.xlsx
@@ -1662,8 +1662,8 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>